<commit_message>
New sample and knit test
</commit_message>
<xml_diff>
--- a/data/full_df.xlsx
+++ b/data/full_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wesleywilliams/Desktop/School/Masters/MThesis/Narrative sign restrictions/Master Thesis/Thesis project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1E92DA-C228-CF45-83BC-BD7FDAD01037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1DE288-F7BC-124D-BD2A-B57C5EE1E28A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="1240" windowWidth="27640" windowHeight="16460" xr2:uid="{1E1B1608-63CF-A641-972A-DF0B9A235901}"/>
   </bookViews>
@@ -1395,7 +1395,7 @@
   <dimension ref="A1:F298"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>